<commit_message>
Se crearon los metodos de validar votante y guardar voto
</commit_message>
<xml_diff>
--- a/ListadoServicios.xlsx
+++ b/ListadoServicios.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>RUTA</t>
   </si>
@@ -37,13 +37,37 @@
   </si>
   <si>
     <t>LISTA TODOS LOS VOTANTES</t>
+  </si>
+  <si>
+    <t>http://192.190.43.117/VotoBack/v1/VotantesService/validarVotante/{cedula}</t>
+  </si>
+  <si>
+    <t>NOTA</t>
+  </si>
+  <si>
+    <t>CUANDO SE INVOQUE ESTE SERVICIO SE ENTENDERA QUE EL VOTANTE PROCEDERA A VOTAR</t>
+  </si>
+  <si>
+    <t>VALIDA SI UN VOTANTE:
+-EXISTE
+-YA ESTA VOTANDO
+-YA VOTÓ</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>GUARDA UN VOTO</t>
+  </si>
+  <si>
+    <t>http://192.190.43.117/VotoBack/v1/VotantesService/guardarVoto/{cedula}/{idCandidato}/{idPuesto}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +84,20 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -82,15 +120,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -369,21 +414,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="94.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="1"/>
+    <col min="4" max="4" width="34.7109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -393,20 +439,54 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>